<commit_message>
merge file admin , lecturer
</commit_message>
<xml_diff>
--- a/src/main/webapp/assets/excel/register_data.xlsx
+++ b/src/main/webapp/assets/excel/register_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project-Final-2023\Final\sci_mju_lifelonglearning\src\main\webapp\assets\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asus\Desktop\sci_mju_lifelonglearning\src\main\webapp\assets\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5D89DA2-48DE-4177-9646-DF92EDF3C6E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCD78FCF-93CB-4AD1-9ACD-57B04911EDE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{0A814F5B-D40A-4EF3-B5C7-5CEF3C53D69A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0A814F5B-D40A-4EF3-B5C7-5CEF3C53D69A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,9 +39,6 @@
     <t>รายชื่อผู้สมัครในหลักสูตร</t>
   </si>
   <si>
-    <t>คณะวิทยาศาสตร์ หมาวิทยาลัยแม้โจ้</t>
-  </si>
-  <si>
     <t>หลักสูตร *************</t>
   </si>
   <si>
@@ -64,6 +61,9 @@
   </si>
   <si>
     <t>สัปดาห์</t>
+  </si>
+  <si>
+    <t>คณะวิทยาศาสตร์ มหาวิทยาลัยแม้โจ้</t>
   </si>
 </sst>
 </file>
@@ -247,7 +247,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -262,20 +262,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -317,7 +309,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="ปกติ" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -388,9 +380,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="ธีม Office 2013 - 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -428,7 +420,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -534,7 +526,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -676,7 +668,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -684,152 +676,151 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5238785-CDB2-43BE-8C1C-8C2475126D25}">
-  <dimension ref="A2:W20"/>
+  <dimension ref="B2:W8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G1048576"/>
+      <selection activeCell="L3" sqref="L3:W3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.6"/>
   <cols>
     <col min="1" max="1" width="6.88671875" style="5" customWidth="1"/>
-    <col min="2" max="2" width="9.77734375" style="8" customWidth="1"/>
-    <col min="3" max="3" width="17.88671875" style="8" customWidth="1"/>
-    <col min="4" max="4" width="31" style="10" customWidth="1"/>
-    <col min="5" max="5" width="17.77734375" style="8" customWidth="1"/>
-    <col min="6" max="6" width="17.88671875" style="8" customWidth="1"/>
-    <col min="7" max="7" width="13.109375" style="8" customWidth="1"/>
-    <col min="8" max="14" width="5.33203125" style="8" customWidth="1"/>
-    <col min="15" max="15" width="5.21875" style="8" customWidth="1"/>
-    <col min="16" max="23" width="5.33203125" style="8" customWidth="1"/>
+    <col min="2" max="2" width="9.77734375" style="6" customWidth="1"/>
+    <col min="3" max="3" width="17.88671875" style="6" customWidth="1"/>
+    <col min="4" max="4" width="31" style="7" customWidth="1"/>
+    <col min="5" max="5" width="17.77734375" style="6" customWidth="1"/>
+    <col min="6" max="6" width="17.88671875" style="6" customWidth="1"/>
+    <col min="7" max="7" width="13.109375" style="6" customWidth="1"/>
+    <col min="8" max="14" width="5.33203125" style="6" customWidth="1"/>
+    <col min="15" max="15" width="5.21875" style="6" customWidth="1"/>
+    <col min="16" max="23" width="5.33203125" style="6" customWidth="1"/>
     <col min="24" max="16384" width="8.88671875" style="5"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:23" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.6"/>
-    <row r="3" spans="1:23" ht="58.2" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A3" s="6"/>
-      <c r="C3" s="13" t="s">
+    <row r="2" spans="2:23" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.6"/>
+    <row r="3" spans="2:23" ht="58.2" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="C3" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="M3" s="8"/>
+      <c r="N3" s="8"/>
+      <c r="O3" s="8"/>
+      <c r="P3" s="8"/>
+      <c r="Q3" s="8"/>
+      <c r="R3" s="8"/>
+      <c r="S3" s="8"/>
+      <c r="T3" s="8"/>
+      <c r="U3" s="8"/>
+      <c r="V3" s="8"/>
+      <c r="W3" s="8"/>
+    </row>
+    <row r="4" spans="2:23" x14ac:dyDescent="0.6">
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="10"/>
+      <c r="L4" s="10"/>
+      <c r="M4" s="10"/>
+      <c r="N4" s="10"/>
+      <c r="O4" s="10"/>
+      <c r="P4" s="10"/>
+      <c r="Q4" s="10"/>
+      <c r="R4" s="10"/>
+      <c r="S4" s="10"/>
+      <c r="T4" s="10"/>
+      <c r="U4" s="10"/>
+      <c r="V4" s="10"/>
+      <c r="W4" s="10"/>
+    </row>
+    <row r="5" spans="2:23" ht="22.2" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="B5" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="13"/>
-      <c r="J3" s="13"/>
-      <c r="K3" s="13"/>
-      <c r="L3" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="M3" s="12"/>
-      <c r="N3" s="12"/>
-      <c r="O3" s="12"/>
-      <c r="P3" s="12"/>
-      <c r="Q3" s="12"/>
-      <c r="R3" s="12"/>
-      <c r="S3" s="12"/>
-      <c r="T3" s="12"/>
-      <c r="U3" s="12"/>
-      <c r="V3" s="12"/>
-      <c r="W3" s="12"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="11"/>
+      <c r="J5" s="11"/>
+      <c r="K5" s="11"/>
+      <c r="L5" s="11"/>
+      <c r="M5" s="11"/>
+      <c r="N5" s="11"/>
+      <c r="O5" s="11"/>
+      <c r="P5" s="11"/>
+      <c r="Q5" s="11"/>
+      <c r="R5" s="11"/>
+      <c r="S5" s="11"/>
+      <c r="T5" s="11"/>
+      <c r="U5" s="11"/>
+      <c r="V5" s="11"/>
+      <c r="W5" s="11"/>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.6">
-      <c r="B4" s="14"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
-      <c r="I4" s="14"/>
-      <c r="J4" s="14"/>
-      <c r="K4" s="14"/>
-      <c r="L4" s="14"/>
-      <c r="M4" s="14"/>
-      <c r="N4" s="14"/>
-      <c r="O4" s="14"/>
-      <c r="P4" s="14"/>
-      <c r="Q4" s="14"/>
-      <c r="R4" s="14"/>
-      <c r="S4" s="14"/>
-      <c r="T4" s="14"/>
-      <c r="U4" s="14"/>
-      <c r="V4" s="14"/>
-      <c r="W4" s="14"/>
+    <row r="6" spans="2:23" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.6"/>
+    <row r="7" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="B7" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="G7" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="H7" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="I7" s="19"/>
+      <c r="J7" s="19"/>
+      <c r="K7" s="19"/>
+      <c r="L7" s="19"/>
+      <c r="M7" s="19"/>
+      <c r="N7" s="19"/>
+      <c r="O7" s="19"/>
+      <c r="P7" s="19"/>
+      <c r="Q7" s="19"/>
+      <c r="R7" s="19"/>
+      <c r="S7" s="19"/>
+      <c r="T7" s="19"/>
+      <c r="U7" s="19"/>
+      <c r="V7" s="19"/>
+      <c r="W7" s="20"/>
     </row>
-    <row r="5" spans="1:23" ht="22.2" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="B5" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" s="15"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="15"/>
-      <c r="H5" s="15"/>
-      <c r="I5" s="15"/>
-      <c r="J5" s="15"/>
-      <c r="K5" s="15"/>
-      <c r="L5" s="15"/>
-      <c r="M5" s="15"/>
-      <c r="N5" s="15"/>
-      <c r="O5" s="15"/>
-      <c r="P5" s="15"/>
-      <c r="Q5" s="15"/>
-      <c r="R5" s="15"/>
-      <c r="S5" s="15"/>
-      <c r="T5" s="15"/>
-      <c r="U5" s="15"/>
-      <c r="V5" s="15"/>
-      <c r="W5" s="15"/>
-    </row>
-    <row r="6" spans="1:23" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.6"/>
-    <row r="7" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="B7" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="E7" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="F7" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="G7" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="H7" s="22" t="s">
-        <v>9</v>
-      </c>
-      <c r="I7" s="23"/>
-      <c r="J7" s="23"/>
-      <c r="K7" s="23"/>
-      <c r="L7" s="23"/>
-      <c r="M7" s="23"/>
-      <c r="N7" s="23"/>
-      <c r="O7" s="23"/>
-      <c r="P7" s="23"/>
-      <c r="Q7" s="23"/>
-      <c r="R7" s="23"/>
-      <c r="S7" s="23"/>
-      <c r="T7" s="23"/>
-      <c r="U7" s="23"/>
-      <c r="V7" s="23"/>
-      <c r="W7" s="24"/>
-    </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.6">
-      <c r="B8" s="17"/>
-      <c r="C8" s="19"/>
-      <c r="D8" s="19"/>
-      <c r="E8" s="19"/>
-      <c r="F8" s="19"/>
-      <c r="G8" s="21"/>
+    <row r="8" spans="2:23" x14ac:dyDescent="0.6">
+      <c r="B8" s="13"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="17"/>
       <c r="H8" s="3">
         <v>1</v>
       </c>
@@ -878,31 +869,6 @@
       <c r="W8" s="1">
         <v>16</v>
       </c>
-    </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.6">
-      <c r="A20" s="7"/>
-      <c r="B20" s="9"/>
-      <c r="C20" s="9"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="9"/>
-      <c r="F20" s="9"/>
-      <c r="G20" s="9"/>
-      <c r="H20" s="9"/>
-      <c r="I20" s="9"/>
-      <c r="J20" s="9"/>
-      <c r="K20" s="9"/>
-      <c r="L20" s="9"/>
-      <c r="M20" s="9"/>
-      <c r="N20" s="9"/>
-      <c r="O20" s="9"/>
-      <c r="P20" s="9"/>
-      <c r="Q20" s="9"/>
-      <c r="R20" s="9"/>
-      <c r="S20" s="9"/>
-      <c r="T20" s="9"/>
-      <c r="U20" s="9"/>
-      <c r="V20" s="9"/>
-      <c r="W20" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="11">

</xml_diff>